<commit_message>
Added "MANAGE" directories for managed documents as per Chandra's advice.
</commit_message>
<xml_diff>
--- a/MGMT/QUALITY/FORMS/SWSYS_TS.xlsx
+++ b/MGMT/QUALITY/FORMS/SWSYS_TS.xlsx
@@ -4,10 +4,10 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="30" windowWidth="18135" windowHeight="7680"/>
+    <workbookView xWindow="480" yWindow="30" windowWidth="18135" windowHeight="7680" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Overview" sheetId="1" r:id="rId1"/>
+    <sheet name="Revision History" sheetId="1" r:id="rId1"/>
     <sheet name="System Test Specifications" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="56">
   <si>
     <t>SERIS</t>
   </si>
@@ -90,9 +90,6 @@
     <t xml:space="preserve">Designation </t>
   </si>
   <si>
-    <t>Document Key:</t>
-  </si>
-  <si>
     <t>Software System Test  Specification and Report</t>
   </si>
   <si>
@@ -109,6 +106,85 @@
   </si>
   <si>
     <t>1.0</t>
+  </si>
+  <si>
+    <t>Test ID</t>
+  </si>
+  <si>
+    <t>Test Objective</t>
+  </si>
+  <si>
+    <t>TestCaseID</t>
+  </si>
+  <si>
+    <t>TestCase Name</t>
+  </si>
+  <si>
+    <t>Tracebility</t>
+  </si>
+  <si>
+    <t>Priority</t>
+  </si>
+  <si>
+    <t>Input</t>
+  </si>
+  <si>
+    <t>Expected Result</t>
+  </si>
+  <si>
+    <t>Test Result</t>
+  </si>
+  <si>
+    <t>Basic initialization of object instance</t>
+  </si>
+  <si>
+    <t>T1.1</t>
+  </si>
+  <si>
+    <t>Object Intialization</t>
+  </si>
+  <si>
+    <t>Initialize  object with known values to its attributes.</t>
+  </si>
+  <si>
+    <t>The object should be initialized with
+the specified values.</t>
+  </si>
+  <si>
+    <t>Pass</t>
+  </si>
+  <si>
+    <t>T1.2</t>
+  </si>
+  <si>
+    <t>T1.3</t>
+  </si>
+  <si>
+    <t>Check object's method functionality</t>
+  </si>
+  <si>
+    <t>T2.1</t>
+  </si>
+  <si>
+    <t>T2.2</t>
+  </si>
+  <si>
+    <t>Fail</t>
+  </si>
+  <si>
+    <t>Numbers of Passed Results</t>
+  </si>
+  <si>
+    <t>Numbers of Failed Results</t>
+  </si>
+  <si>
+    <t>Numbers of No-Results</t>
+  </si>
+  <si>
+    <t>Test-1 16-08-2018</t>
+  </si>
+  <si>
+    <t>NoResult</t>
   </si>
 </sst>
 </file>
@@ -153,7 +229,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -184,6 +260,36 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF5050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="10">
     <border>
@@ -304,38 +410,14 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -345,6 +427,50 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -379,7 +505,7 @@
         <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:lc="http://schemas.openxmlformats.org/drawingml/2006/lockedCanvas" xmlns:pic="http://schemas.openxmlformats.org/drawingml/2006/picture" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns:wps="http://schemas.microsoft.com/office/word/2010/wordprocessingShape" xmlns:wne="http://schemas.microsoft.com/office/word/2006/wordml" xmlns:wpi="http://schemas.microsoft.com/office/word/2010/wordprocessingInk" xmlns:wpg="http://schemas.microsoft.com/office/word/2010/wordprocessingGroup" xmlns:w16se="http://schemas.microsoft.com/office/word/2015/wordml/symex" xmlns:w16cid="http://schemas.microsoft.com/office/word/2016/wordml/cid" xmlns:w15="http://schemas.microsoft.com/office/word/2012/wordml" xmlns:w14="http://schemas.microsoft.com/office/word/2010/wordml" xmlns:w="http://schemas.openxmlformats.org/wordprocessingml/2006/main" xmlns:w10="urn:schemas-microsoft-com:office:word" xmlns:wp="http://schemas.openxmlformats.org/drawingml/2006/wordprocessingDrawing" xmlns:wp14="http://schemas.microsoft.com/office/word/2010/wordprocessingDrawing" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math" xmlns:o="urn:schemas-microsoft-com:office:office" xmlns:am3d="http://schemas.microsoft.com/office/drawing/2017/model3d" xmlns:aink="http://schemas.microsoft.com/office/drawing/2016/ink" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:cx8="http://schemas.microsoft.com/office/drawing/2016/5/14/chartex" xmlns:cx7="http://schemas.microsoft.com/office/drawing/2016/5/13/chartex" xmlns:cx6="http://schemas.microsoft.com/office/drawing/2016/5/12/chartex" xmlns:cx5="http://schemas.microsoft.com/office/drawing/2016/5/11/chartex" xmlns:cx4="http://schemas.microsoft.com/office/drawing/2016/5/10/chartex" xmlns:cx3="http://schemas.microsoft.com/office/drawing/2016/5/9/chartex" xmlns:cx2="http://schemas.microsoft.com/office/drawing/2015/10/21/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:wpc="http://schemas.microsoft.com/office/word/2010/wordprocessingCanvas" xmlns="" val="0"/>
+              <a14:useLocalDpi xmlns="" xmlns:wpc="http://schemas.microsoft.com/office/word/2010/wordprocessingCanvas" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:cx2="http://schemas.microsoft.com/office/drawing/2015/10/21/chartex" xmlns:cx3="http://schemas.microsoft.com/office/drawing/2016/5/9/chartex" xmlns:cx4="http://schemas.microsoft.com/office/drawing/2016/5/10/chartex" xmlns:cx5="http://schemas.microsoft.com/office/drawing/2016/5/11/chartex" xmlns:cx6="http://schemas.microsoft.com/office/drawing/2016/5/12/chartex" xmlns:cx7="http://schemas.microsoft.com/office/drawing/2016/5/13/chartex" xmlns:cx8="http://schemas.microsoft.com/office/drawing/2016/5/14/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:aink="http://schemas.microsoft.com/office/drawing/2016/ink" xmlns:am3d="http://schemas.microsoft.com/office/drawing/2017/model3d" xmlns:o="urn:schemas-microsoft-com:office:office" xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:wp14="http://schemas.microsoft.com/office/word/2010/wordprocessingDrawing" xmlns:wp="http://schemas.openxmlformats.org/drawingml/2006/wordprocessingDrawing" xmlns:w10="urn:schemas-microsoft-com:office:word" xmlns:w="http://schemas.openxmlformats.org/wordprocessingml/2006/main" xmlns:w14="http://schemas.microsoft.com/office/word/2010/wordml" xmlns:w15="http://schemas.microsoft.com/office/word/2012/wordml" xmlns:w16cid="http://schemas.microsoft.com/office/word/2016/wordml/cid" xmlns:w16se="http://schemas.microsoft.com/office/word/2015/wordml/symex" xmlns:wpg="http://schemas.microsoft.com/office/word/2010/wordprocessingGroup" xmlns:wpi="http://schemas.microsoft.com/office/word/2010/wordprocessingInk" xmlns:wne="http://schemas.microsoft.com/office/word/2006/wordml" xmlns:wps="http://schemas.microsoft.com/office/word/2010/wordprocessingShape" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns:pic="http://schemas.openxmlformats.org/drawingml/2006/picture" xmlns:lc="http://schemas.openxmlformats.org/drawingml/2006/lockedCanvas" val="0"/>
             </a:ext>
           </a:extLst>
         </a:blip>
@@ -694,8 +820,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A4:D41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G36" sqref="G36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -708,7 +834,7 @@
   <sheetData>
     <row r="4" spans="1:3">
       <c r="A4" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
@@ -720,7 +846,7 @@
     </row>
     <row r="9" spans="1:3">
       <c r="A9" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B9" s="1"/>
     </row>
@@ -736,8 +862,8 @@
       <c r="A13" t="s">
         <v>3</v>
       </c>
-      <c r="B13" s="20" t="s">
-        <v>30</v>
+      <c r="B13" s="8" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="14" spans="1:3">
@@ -753,7 +879,7 @@
         <v>6</v>
       </c>
       <c r="B15" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="18" spans="1:4">
@@ -776,8 +902,8 @@
       </c>
     </row>
     <row r="20" spans="1:4">
-      <c r="A20" s="19" t="s">
-        <v>29</v>
+      <c r="A20" s="7" t="s">
+        <v>28</v>
       </c>
       <c r="B20" s="4" t="s">
         <v>12</v>
@@ -790,8 +916,8 @@
       </c>
     </row>
     <row r="21" spans="1:4">
-      <c r="A21" s="21" t="s">
-        <v>30</v>
+      <c r="A21" s="9" t="s">
+        <v>29</v>
       </c>
       <c r="B21" s="4" t="s">
         <v>12</v>
@@ -876,10 +1002,10 @@
       <c r="D33" s="3"/>
     </row>
     <row r="36" spans="1:4">
-      <c r="A36" s="5" t="s">
+      <c r="A36" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="B36" s="6"/>
+      <c r="B36" s="11"/>
       <c r="C36" s="2" t="s">
         <v>9</v>
       </c>
@@ -888,66 +1014,63 @@
       </c>
     </row>
     <row r="37" spans="1:4">
-      <c r="A37" s="7" t="s">
+      <c r="A37" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="B37" s="8" t="s">
+      <c r="B37" s="6" t="s">
         <v>18</v>
       </c>
       <c r="C37" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="D37" s="7" t="s">
+      <c r="D37" s="5" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="38" spans="1:4">
-      <c r="A38" s="7" t="s">
+      <c r="A38" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="B38" s="8" t="s">
+      <c r="B38" s="6" t="s">
         <v>18</v>
       </c>
       <c r="C38" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="D38" s="7" t="s">
+      <c r="D38" s="5" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="39" spans="1:4">
-      <c r="A39" s="9" t="s">
+      <c r="A39" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="B39" s="10"/>
-      <c r="C39" s="11" t="s">
+      <c r="B39" s="13"/>
+      <c r="C39" s="18" t="s">
         <v>23</v>
       </c>
-      <c r="D39" s="12"/>
+      <c r="D39" s="19"/>
     </row>
     <row r="40" spans="1:4">
-      <c r="A40" s="13"/>
-      <c r="B40" s="14"/>
-      <c r="C40" s="15" t="s">
-        <v>27</v>
-      </c>
-      <c r="D40" s="16"/>
+      <c r="A40" s="14"/>
+      <c r="B40" s="15"/>
+      <c r="C40" s="30" t="s">
+        <v>26</v>
+      </c>
+      <c r="D40" s="31"/>
     </row>
     <row r="41" spans="1:4">
-      <c r="A41" s="17"/>
-      <c r="B41" s="18"/>
-      <c r="C41" s="15" t="s">
-        <v>24</v>
-      </c>
-      <c r="D41" s="16"/>
+      <c r="A41" s="16"/>
+      <c r="B41" s="17"/>
+      <c r="C41" s="32"/>
+      <c r="D41" s="33"/>
     </row>
   </sheetData>
-  <mergeCells count="5">
+  <mergeCells count="4">
     <mergeCell ref="A36:B36"/>
     <mergeCell ref="A39:B41"/>
     <mergeCell ref="C39:D39"/>
-    <mergeCell ref="C40:D40"/>
-    <mergeCell ref="C41:D41"/>
+    <mergeCell ref="C40:D41"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="B37" r:id="rId1"/>
@@ -961,14 +1084,510 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A1:R35"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="M35" sqref="M35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="8.28515625" customWidth="1"/>
+    <col min="2" max="2" width="37.5703125" customWidth="1"/>
+    <col min="3" max="3" width="13.42578125" customWidth="1"/>
+    <col min="4" max="4" width="20.140625" customWidth="1"/>
+    <col min="5" max="5" width="11.140625" customWidth="1"/>
+    <col min="6" max="6" width="10.85546875" customWidth="1"/>
+    <col min="7" max="7" width="33.85546875" customWidth="1"/>
+    <col min="8" max="8" width="42.7109375" customWidth="1"/>
+    <col min="9" max="9" width="18.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:18">
+      <c r="A1" s="20" t="s">
+        <v>30</v>
+      </c>
+      <c r="B1" s="20" t="s">
+        <v>31</v>
+      </c>
+      <c r="C1" s="20" t="s">
+        <v>32</v>
+      </c>
+      <c r="D1" s="20" t="s">
+        <v>33</v>
+      </c>
+      <c r="E1" s="20" t="s">
+        <v>34</v>
+      </c>
+      <c r="F1" s="20" t="s">
+        <v>35</v>
+      </c>
+      <c r="G1" s="20" t="s">
+        <v>36</v>
+      </c>
+      <c r="H1" s="20" t="s">
+        <v>37</v>
+      </c>
+      <c r="I1" s="20" t="s">
+        <v>38</v>
+      </c>
+      <c r="P1" s="29" t="s">
+        <v>44</v>
+      </c>
+      <c r="Q1" s="29" t="s">
+        <v>50</v>
+      </c>
+      <c r="R1" s="29" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18">
+      <c r="A2" s="21"/>
+      <c r="B2" s="21"/>
+      <c r="C2" s="21"/>
+      <c r="D2" s="21"/>
+      <c r="E2" s="21"/>
+      <c r="F2" s="21"/>
+      <c r="G2" s="21"/>
+      <c r="H2" s="21"/>
+      <c r="I2" s="22" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" ht="30.75" customHeight="1">
+      <c r="A3" s="3">
+        <v>1</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="C3" s="23" t="s">
+        <v>40</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="E3" s="3"/>
+      <c r="F3" s="3">
+        <v>1</v>
+      </c>
+      <c r="G3" s="24" t="s">
+        <v>42</v>
+      </c>
+      <c r="H3" s="24" t="s">
+        <v>43</v>
+      </c>
+      <c r="I3" s="25" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18">
+      <c r="A4" s="3"/>
+      <c r="B4" s="3"/>
+      <c r="C4" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="D4" s="3"/>
+      <c r="E4" s="3"/>
+      <c r="F4" s="3">
+        <v>1</v>
+      </c>
+      <c r="G4" s="3"/>
+      <c r="H4" s="3"/>
+      <c r="I4" s="25" t="s">
+        <v>44</v>
+      </c>
+      <c r="P4" s="29"/>
+      <c r="Q4" s="29"/>
+      <c r="R4" s="29"/>
+    </row>
+    <row r="5" spans="1:18">
+      <c r="A5" s="3"/>
+      <c r="B5" s="3"/>
+      <c r="C5" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="D5" s="3"/>
+      <c r="E5" s="3"/>
+      <c r="F5" s="3">
+        <v>1</v>
+      </c>
+      <c r="G5" s="3"/>
+      <c r="H5" s="3"/>
+      <c r="I5" s="25" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18">
+      <c r="A6" s="3">
+        <v>2</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="D6" s="3"/>
+      <c r="E6" s="3"/>
+      <c r="F6" s="3">
+        <v>2</v>
+      </c>
+      <c r="G6" s="3"/>
+      <c r="H6" s="3"/>
+      <c r="I6" s="25" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18">
+      <c r="A7" s="3"/>
+      <c r="B7" s="3"/>
+      <c r="C7" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="D7" s="3"/>
+      <c r="E7" s="3"/>
+      <c r="F7" s="3">
+        <v>1</v>
+      </c>
+      <c r="G7" s="3"/>
+      <c r="H7" s="3"/>
+      <c r="I7" s="25" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18">
+      <c r="A8" s="3"/>
+      <c r="B8" s="3"/>
+      <c r="C8" s="3"/>
+      <c r="D8" s="3"/>
+      <c r="E8" s="3"/>
+      <c r="F8" s="3"/>
+      <c r="G8" s="3"/>
+      <c r="H8" s="3"/>
+      <c r="I8" s="25" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18">
+      <c r="A9" s="3"/>
+      <c r="B9" s="3"/>
+      <c r="C9" s="3"/>
+      <c r="D9" s="3"/>
+      <c r="E9" s="3"/>
+      <c r="F9" s="3"/>
+      <c r="G9" s="3"/>
+      <c r="H9" s="3"/>
+      <c r="I9" s="25" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18">
+      <c r="A10" s="3"/>
+      <c r="B10" s="3"/>
+      <c r="C10" s="3"/>
+      <c r="D10" s="3"/>
+      <c r="E10" s="3"/>
+      <c r="F10" s="3"/>
+      <c r="G10" s="3"/>
+      <c r="H10" s="3"/>
+      <c r="I10" s="25" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18">
+      <c r="A11" s="3"/>
+      <c r="B11" s="3"/>
+      <c r="C11" s="3"/>
+      <c r="D11" s="3"/>
+      <c r="E11" s="3"/>
+      <c r="F11" s="3"/>
+      <c r="G11" s="3"/>
+      <c r="H11" s="3"/>
+      <c r="I11" s="25" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="12" spans="1:18">
+      <c r="A12" s="3"/>
+      <c r="B12" s="3"/>
+      <c r="C12" s="3"/>
+      <c r="D12" s="3"/>
+      <c r="E12" s="3"/>
+      <c r="F12" s="3"/>
+      <c r="G12" s="3"/>
+      <c r="H12" s="3"/>
+      <c r="I12" s="25" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18">
+      <c r="A13" s="3"/>
+      <c r="B13" s="3"/>
+      <c r="C13" s="3"/>
+      <c r="D13" s="3"/>
+      <c r="E13" s="3"/>
+      <c r="F13" s="3"/>
+      <c r="G13" s="3"/>
+      <c r="H13" s="3"/>
+      <c r="I13" s="25" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="14" spans="1:18">
+      <c r="A14" s="3"/>
+      <c r="B14" s="3"/>
+      <c r="C14" s="3"/>
+      <c r="D14" s="3"/>
+      <c r="E14" s="3"/>
+      <c r="F14" s="3"/>
+      <c r="G14" s="3"/>
+      <c r="H14" s="3"/>
+      <c r="I14" s="25" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="15" spans="1:18">
+      <c r="A15" s="3"/>
+      <c r="B15" s="3"/>
+      <c r="C15" s="3"/>
+      <c r="D15" s="3"/>
+      <c r="E15" s="3"/>
+      <c r="F15" s="3"/>
+      <c r="G15" s="3"/>
+      <c r="H15" s="3"/>
+      <c r="I15" s="25" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="16" spans="1:18">
+      <c r="A16" s="3"/>
+      <c r="B16" s="3"/>
+      <c r="C16" s="3"/>
+      <c r="D16" s="3"/>
+      <c r="E16" s="3"/>
+      <c r="F16" s="3"/>
+      <c r="G16" s="3"/>
+      <c r="H16" s="3"/>
+      <c r="I16" s="25" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9">
+      <c r="A17" s="3"/>
+      <c r="B17" s="3"/>
+      <c r="C17" s="3"/>
+      <c r="D17" s="3"/>
+      <c r="E17" s="3"/>
+      <c r="F17" s="3"/>
+      <c r="G17" s="3"/>
+      <c r="H17" s="3"/>
+      <c r="I17" s="25" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9">
+      <c r="A18" s="3"/>
+      <c r="B18" s="3"/>
+      <c r="C18" s="3"/>
+      <c r="D18" s="3"/>
+      <c r="E18" s="3"/>
+      <c r="F18" s="3"/>
+      <c r="G18" s="3"/>
+      <c r="H18" s="3"/>
+      <c r="I18" s="25" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9">
+      <c r="A19" s="3"/>
+      <c r="B19" s="3"/>
+      <c r="C19" s="3"/>
+      <c r="D19" s="3"/>
+      <c r="E19" s="3"/>
+      <c r="F19" s="3"/>
+      <c r="G19" s="3"/>
+      <c r="H19" s="3"/>
+      <c r="I19" s="25" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9">
+      <c r="A20" s="3"/>
+      <c r="B20" s="3"/>
+      <c r="C20" s="3"/>
+      <c r="D20" s="3"/>
+      <c r="E20" s="3"/>
+      <c r="F20" s="3"/>
+      <c r="G20" s="3"/>
+      <c r="H20" s="3"/>
+      <c r="I20" s="25" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9">
+      <c r="A21" s="3"/>
+      <c r="B21" s="3"/>
+      <c r="C21" s="3"/>
+      <c r="D21" s="3"/>
+      <c r="E21" s="3"/>
+      <c r="F21" s="3"/>
+      <c r="G21" s="3"/>
+      <c r="H21" s="3"/>
+      <c r="I21" s="25" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9">
+      <c r="A22" s="3"/>
+      <c r="B22" s="3"/>
+      <c r="C22" s="3"/>
+      <c r="D22" s="3"/>
+      <c r="E22" s="3"/>
+      <c r="F22" s="3"/>
+      <c r="G22" s="3"/>
+      <c r="H22" s="3"/>
+      <c r="I22" s="25" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9">
+      <c r="A23" s="3"/>
+      <c r="B23" s="3"/>
+      <c r="C23" s="3"/>
+      <c r="D23" s="3"/>
+      <c r="E23" s="3"/>
+      <c r="F23" s="3"/>
+      <c r="G23" s="3"/>
+      <c r="H23" s="3"/>
+      <c r="I23" s="25" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9">
+      <c r="A24" s="3"/>
+      <c r="B24" s="3"/>
+      <c r="C24" s="3"/>
+      <c r="D24" s="3"/>
+      <c r="E24" s="3"/>
+      <c r="F24" s="3"/>
+      <c r="G24" s="3"/>
+      <c r="H24" s="3"/>
+      <c r="I24" s="25" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9">
+      <c r="A25" s="3"/>
+      <c r="B25" s="3"/>
+      <c r="C25" s="3"/>
+      <c r="D25" s="3"/>
+      <c r="E25" s="3"/>
+      <c r="F25" s="3"/>
+      <c r="G25" s="3"/>
+      <c r="H25" s="3"/>
+      <c r="I25" s="25" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9">
+      <c r="A26" s="3"/>
+      <c r="B26" s="3"/>
+      <c r="C26" s="3"/>
+      <c r="D26" s="3"/>
+      <c r="E26" s="3"/>
+      <c r="F26" s="3"/>
+      <c r="G26" s="3"/>
+      <c r="H26" s="3"/>
+      <c r="I26" s="25" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9">
+      <c r="A27" s="3"/>
+      <c r="B27" s="3"/>
+      <c r="C27" s="3"/>
+      <c r="D27" s="3"/>
+      <c r="E27" s="3"/>
+      <c r="F27" s="3"/>
+      <c r="G27" s="3"/>
+      <c r="H27" s="3"/>
+      <c r="I27" s="25" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9">
+      <c r="A28" s="3"/>
+      <c r="B28" s="3"/>
+      <c r="C28" s="3"/>
+      <c r="D28" s="3"/>
+      <c r="E28" s="3"/>
+      <c r="F28" s="3"/>
+      <c r="G28" s="3"/>
+      <c r="H28" s="3"/>
+      <c r="I28" s="25" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9">
+      <c r="A29" s="3"/>
+      <c r="B29" s="3"/>
+      <c r="C29" s="3"/>
+      <c r="D29" s="3"/>
+      <c r="E29" s="3"/>
+      <c r="F29" s="3"/>
+      <c r="G29" s="3"/>
+      <c r="H29" s="3"/>
+      <c r="I29" s="25" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9">
+      <c r="A30" s="3"/>
+      <c r="B30" s="3"/>
+      <c r="C30" s="3"/>
+      <c r="D30" s="3"/>
+      <c r="E30" s="3"/>
+      <c r="F30" s="3"/>
+      <c r="G30" s="3"/>
+      <c r="H30" s="3"/>
+      <c r="I30" s="25" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="33" spans="8:9">
+      <c r="H33" s="26" t="s">
+        <v>51</v>
+      </c>
+      <c r="I33" s="27">
+        <f>IF(I3=P1,1,0)+IF(I4=P1,1,0)+IF(I5=P1,1,0)+IF(I6=P1,1,0)+IF(I7=P1,1,0)+IF(I8=P1,1,0)+IF(I9=P1,1,0)+IF(I10=P1,1,0)+IF(I11=P1,1,0)+IF(I12=P1,1,0)+IF(I13=P1,1,0)+IF(I14=P1,1,0)+IF(I15=P1,1,0)+IF(I16=P1,1,0)+IF(I17=P1,1,0)+IF(I18=P1,1,0)+IF(I19=P1,1,0)+IF(I20=P1,1,0)+IF(I21=P1,1,0)+IF(I22=P1,1,0)+IF(I23=P1,1,0)+IF(I24=P1,1,0)+IF(I25=P1,1,0)+IF(I26=P1,1,0)+IF(I27=P1,1,0)+IF(I28=P1,1,0)+IF(I29=P1,1,0)+IF(I30=P1,1,0)</f>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="34" spans="8:9">
+      <c r="H34" s="26" t="s">
+        <v>52</v>
+      </c>
+      <c r="I34" s="28">
+        <f>IF(I3=Q1,1,0)+IF(I4=Q1,1,0)+IF(I5=Q1,1,0)+IF(I6=Q1,1,0)+IF(I7=Q1,1,0)+IF(I8=Q1,1,0)+IF(I9=Q1,1,0)+IF(I10=Q1,1,0)+IF(I11=Q1,1,0)+IF(I12=Q1,1,0)+IF(I13=Q1,1,0)+IF(I14=Q1,1,0)+IF(I15=Q1,1,0)+IF(I16=Q1,1,0)+IF(I17=Q1,1,0)+IF(I18=Q1,1,0)+IF(I19=Q1,1,0)+IF(I20=Q1,1,0)+IF(I21=Q1,1,0)+IF(I22=Q1,1,0)+IF(I23=Q1,1,0)+IF(I24=Q1,1,0)+IF(I25=Q1,1,0)+IF(I26=Q1,1,0)+IF(I27=Q1,1,0)+IF(I28=Q1,1,0)+IF(I29=Q1,1,0)+IF(I30=Q1,1,0)</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="35" spans="8:9">
+      <c r="H35" s="26" t="s">
+        <v>53</v>
+      </c>
+      <c r="I35" s="2"/>
+    </row>
+  </sheetData>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I3:I30">
+      <formula1>$P$1:$R$1</formula1>
+    </dataValidation>
+  </dataValidations>
+  <hyperlinks>
+    <hyperlink ref="I2" location="'Test-1 15-03-2017'!A1" display="Test-1 15-03-2017"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>